<commit_message>
cv subarea estimates added
</commit_message>
<xml_diff>
--- a/RESULTS/Table_4_summary_abundance.xlsx
+++ b/RESULTS/Table_4_summary_abundance.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t xml:space="preserve">0.1714 (0.0393 - 0.3258)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cv area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5519 (815 - 11397)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0086 (0.0013 - 0.0177)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.069 (0.0102 - 0.1424)</t>
   </si>
 </sst>
 </file>
@@ -433,6 +445,23 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="n">
+        <v>80025</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
added estimate and  ci for maximum density in table 4
</commit_message>
<xml_diff>
--- a/RESULTS/Table_4_summary_abundance.xlsx
+++ b/RESULTS/Table_4_summary_abundance.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -29,6 +29,9 @@
     <t xml:space="preserve">D_95CI</t>
   </si>
   <si>
+    <t xml:space="preserve">dmax_95CI</t>
+  </si>
+  <si>
     <t xml:space="preserve">survey area</t>
   </si>
   <si>
@@ -39,6 +42,9 @@
   </si>
   <si>
     <t xml:space="preserve">0.0194 (0.0025 - 0.0432)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4188 (0.2205 - 0.6171)</t>
   </si>
   <si>
     <t xml:space="preserve">hotspots</t>
@@ -410,56 +416,68 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
         <v>319812.5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="n">
         <v>20381.25</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="n">
         <v>80025</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>